<commit_message>
update lai khoa,lop; them nut tim kiem lop
</commit_message>
<xml_diff>
--- a/DataSinhVien.xlsx
+++ b/DataSinhVien.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.NET\ThucTapCoSoNganh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThucTapCoSoNganhGit\ThucTapCoSoNganh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FA13A6-1300-4B8F-8A4D-F58B5E9E7780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E06FC6-E2A8-4477-9930-B2AA55CFC61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB55097F-133D-4C6C-982C-3FB5870A35D5}"/>
   </bookViews>
@@ -122,7 +122,7 @@
     <t>anh</t>
   </si>
   <si>
-    <t>""</t>
+    <t>"C:\Users\KHANH\Downloads\VuDinhDuc.jpg"</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +519,7 @@
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>